<commit_message>
Water Project Fix small bug
</commit_message>
<xml_diff>
--- a/assets/water/meter_import.xlsx
+++ b/assets/water/meter_import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loatchoeun/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/htdocs/c2/assets/water/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>number</t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t>date_used</t>
+  </si>
+  <si>
+    <t>deposit</t>
+  </si>
+  <si>
+    <t>balance</t>
   </si>
 </sst>
 </file>
@@ -425,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -438,7 +444,7 @@
     <col min="7" max="7" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,8 +469,14 @@
       <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
fix dashboard utiblil choeun
</commit_message>
<xml_diff>
--- a/assets/water/meter_import.xlsx
+++ b/assets/water/meter_import.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/htdocs/c2/assets/water/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="26240" yWindow="460" windowWidth="24960" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="meter" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -70,9 +65,6 @@
     <t>start_up</t>
   </si>
   <si>
-    <t>customer</t>
-  </si>
-  <si>
     <t>bloc</t>
   </si>
   <si>
@@ -98,6 +90,9 @@
   </si>
   <si>
     <t>balance</t>
+  </si>
+  <si>
+    <t>property</t>
   </si>
 </sst>
 </file>
@@ -211,7 +206,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -246,7 +241,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -423,7 +418,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -434,17 +429,17 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="4" max="4" width="18.1640625" customWidth="1"/>
     <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,30 +450,30 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
         <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -487,10 +482,10 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -505,5 +500,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
contact group sort by name
</commit_message>
<xml_diff>
--- a/assets/water/meter_import.xlsx
+++ b/assets/water/meter_import.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="6260" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="meter" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>number</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>multiplier</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>active/inactive/void</t>
   </si>
 </sst>
 </file>
@@ -210,8 +216,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -228,15 +236,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -504,7 +514,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -512,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -523,9 +533,10 @@
     <col min="4" max="4" width="18.1640625" customWidth="1"/>
     <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.1640625" customWidth="1"/>
+    <col min="18" max="18" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -577,8 +588,11 @@
       <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" ht="25">
+    <row r="2" spans="1:18" ht="17">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -626,6 +640,9 @@
       </c>
       <c r="Q2" t="s">
         <v>15</v>
+      </c>
+      <c r="R2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>